<commit_message>
revb mostly finished, need to add BLE chip
</commit_message>
<xml_diff>
--- a/hardware/eagle/bbb-cc2520/rev_b/bbb-cc2520_b_bom.xlsx
+++ b/hardware/eagle/bbb-cc2520/rev_b/bbb-cc2520_b_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Work-Lab11\beaglebone-cc2520\hardware\eagle\bbb-cc2520\rev_a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Work-Lab11\beaglebone-cc2520\hardware\eagle\bbb-cc2520\rev_b\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -117,9 +117,6 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
     <t>RESISTOR, American symbol</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>1276-4083-1-ND</t>
+  </si>
+  <si>
+    <t>R12, R18, R19</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,16 +1492,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1509,27 +1509,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
@@ -1547,21 +1547,21 @@
         <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
@@ -1578,18 +1578,18 @@
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1610,7 +1610,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
@@ -1618,7 +1618,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
@@ -1636,21 +1636,21 @@
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1658,27 +1658,27 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -1687,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -1696,21 +1696,21 @@
         <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>26</v>
@@ -1727,21 +1727,21 @@
         <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -1758,21 +1758,21 @@
         <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>26</v>
@@ -1789,21 +1789,21 @@
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
@@ -1820,18 +1820,18 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K12" s="1"/>
     </row>
@@ -1840,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -1849,21 +1849,21 @@
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1946,19 +1946,19 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>9</v>
@@ -1973,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -1982,18 +1982,18 @@
         <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K18" s="1"/>
     </row>
@@ -2002,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -2011,18 +2011,18 @@
         <v>21</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="1"/>
       <c r="J19" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K19" s="1"/>
     </row>
@@ -2031,7 +2031,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
@@ -2040,18 +2040,18 @@
         <v>21</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K20" s="1"/>
     </row>
@@ -2072,15 +2072,15 @@
         <v>22</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K21" s="1"/>
     </row>
@@ -2101,15 +2101,15 @@
         <v>24</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="1"/>
       <c r="J22" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K22" s="1"/>
     </row>
@@ -2118,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>20</v>
@@ -2127,18 +2127,18 @@
         <v>21</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K23" s="1"/>
     </row>
@@ -2147,22 +2147,22 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2174,26 +2174,26 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2212,13 +2212,13 @@
         <v>31</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2230,7 +2230,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>
@@ -2239,13 +2239,13 @@
         <v>31</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2266,13 +2266,13 @@
         <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2284,7 +2284,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>30</v>
@@ -2293,13 +2293,13 @@
         <v>31</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -2320,13 +2320,13 @@
         <v>31</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2338,7 +2338,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -2347,13 +2347,13 @@
         <v>31</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2365,7 +2365,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>30</v>
@@ -2374,13 +2374,13 @@
         <v>31</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2392,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>30</v>
@@ -2401,13 +2401,13 @@
         <v>31</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2419,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>30</v>
@@ -2428,13 +2428,13 @@
         <v>31</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2446,22 +2446,22 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2473,22 +2473,22 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="F36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="1"/>
@@ -2500,22 +2500,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="1"/>
@@ -2527,25 +2527,25 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2556,22 +2556,22 @@
         <v>2</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>

</xml_diff>